<commit_message>
Add GraphVisualizer and GraphLoader with MST visualization
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -141,7 +141,7 @@
         <v>26.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>4.3521</v>
+        <v>3.5934</v>
       </c>
     </row>
     <row r="3">
@@ -164,7 +164,7 @@
         <v>72.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>1.8798</v>
+        <v>3.3008</v>
       </c>
     </row>
     <row r="4">
@@ -187,7 +187,7 @@
         <v>10.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>0.1315</v>
+        <v>0.1131</v>
       </c>
     </row>
     <row r="5">
@@ -210,7 +210,7 @@
         <v>36.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>0.0687</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="6">
@@ -233,7 +233,7 @@
         <v>7.0</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>0.1364</v>
+        <v>0.1108</v>
       </c>
     </row>
     <row r="7">
@@ -256,7 +256,7 @@
         <v>28.0</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>0.0435</v>
+        <v>0.0441</v>
       </c>
     </row>
     <row r="8">
@@ -279,7 +279,7 @@
         <v>19.0</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>0.0998</v>
+        <v>0.1109</v>
       </c>
     </row>
     <row r="9">
@@ -302,7 +302,7 @@
         <v>52.0</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>0.0676</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="10">
@@ -325,7 +325,7 @@
         <v>58.0</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>0.2987</v>
+        <v>0.2542</v>
       </c>
     </row>
     <row r="11">
@@ -348,7 +348,7 @@
         <v>116.0</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>0.2132</v>
+        <v>0.1812</v>
       </c>
     </row>
     <row r="12">
@@ -371,7 +371,7 @@
         <v>598.0</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>3.8234</v>
+        <v>3.3341</v>
       </c>
     </row>
     <row r="13">
@@ -394,7 +394,7 @@
         <v>1196.0</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>2.9948</v>
+        <v>1.3333</v>
       </c>
     </row>
     <row r="14">
@@ -417,7 +417,7 @@
         <v>564.0</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>9.7924</v>
+        <v>1.1453</v>
       </c>
     </row>
     <row r="15">
@@ -440,7 +440,7 @@
         <v>1128.0</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>2.4115</v>
+        <v>1.0004</v>
       </c>
     </row>
     <row r="16">
@@ -463,7 +463,7 @@
         <v>160.0</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>0.9199</v>
+        <v>0.2728</v>
       </c>
     </row>
     <row r="17">
@@ -486,7 +486,7 @@
         <v>320.0</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>0.5852</v>
+        <v>0.2563</v>
       </c>
     </row>
     <row r="18">
@@ -509,7 +509,7 @@
         <v>430.0</v>
       </c>
       <c r="G18" t="n" s="0">
-        <v>1.9764</v>
+        <v>0.659</v>
       </c>
     </row>
     <row r="19">
@@ -532,7 +532,7 @@
         <v>860.0</v>
       </c>
       <c r="G19" t="n" s="0">
-        <v>1.8912</v>
+        <v>0.646</v>
       </c>
     </row>
     <row r="20">
@@ -543,7 +543,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>3891.0</v>
+        <v>3911.0</v>
       </c>
       <c r="D20" t="n" s="0">
         <v>157.0</v>
@@ -552,10 +552,10 @@
         <v>314.0</v>
       </c>
       <c r="F20" t="n" s="0">
-        <v>313.0</v>
+        <v>314.0</v>
       </c>
       <c r="G20" t="n" s="0">
-        <v>1.624</v>
+        <v>0.5927</v>
       </c>
     </row>
     <row r="21">
@@ -578,7 +578,7 @@
         <v>628.0</v>
       </c>
       <c r="G21" t="n" s="0">
-        <v>1.4699</v>
+        <v>0.4664</v>
       </c>
     </row>
     <row r="22">
@@ -601,7 +601,7 @@
         <v>159.0</v>
       </c>
       <c r="G22" t="n" s="0">
-        <v>0.6816</v>
+        <v>0.2838</v>
       </c>
     </row>
     <row r="23">
@@ -624,7 +624,7 @@
         <v>360.0</v>
       </c>
       <c r="G23" t="n" s="0">
-        <v>0.6414</v>
+        <v>0.2725</v>
       </c>
     </row>
     <row r="24">
@@ -635,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C24" t="n" s="0">
-        <v>6874.0</v>
+        <v>6935.0</v>
       </c>
       <c r="D24" t="n" s="0">
         <v>252.0</v>
@@ -644,10 +644,10 @@
         <v>504.0</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>503.0</v>
+        <v>504.0</v>
       </c>
       <c r="G24" t="n" s="0">
-        <v>1.0979</v>
+        <v>0.7085</v>
       </c>
     </row>
     <row r="25">
@@ -670,7 +670,7 @@
         <v>1008.0</v>
       </c>
       <c r="G25" t="n" s="0">
-        <v>1.0344</v>
+        <v>0.699</v>
       </c>
     </row>
     <row r="26">
@@ -693,7 +693,7 @@
         <v>524.0</v>
       </c>
       <c r="G26" t="n" s="0">
-        <v>1.1373</v>
+        <v>1.0056</v>
       </c>
     </row>
     <row r="27">
@@ -716,7 +716,7 @@
         <v>1048.0</v>
       </c>
       <c r="G27" t="n" s="0">
-        <v>1.0127</v>
+        <v>0.9665</v>
       </c>
     </row>
     <row r="28">
@@ -727,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="C28" t="n" s="0">
-        <v>0.0</v>
+        <v>5609.0</v>
       </c>
       <c r="D28" t="n" s="0">
         <v>195.0</v>
@@ -736,10 +736,10 @@
         <v>390.0</v>
       </c>
       <c r="F28" t="n" s="0">
-        <v>0.0</v>
+        <v>390.0</v>
       </c>
       <c r="G28" t="n" s="0">
-        <v>0.3028</v>
+        <v>0.8486</v>
       </c>
     </row>
     <row r="29">
@@ -762,7 +762,7 @@
         <v>780.0</v>
       </c>
       <c r="G29" t="n" s="0">
-        <v>0.7141</v>
+        <v>0.6419</v>
       </c>
     </row>
     <row r="30">
@@ -785,7 +785,7 @@
         <v>264.0</v>
       </c>
       <c r="G30" t="n" s="0">
-        <v>0.4652</v>
+        <v>0.5675</v>
       </c>
     </row>
     <row r="31">
@@ -808,7 +808,7 @@
         <v>528.0</v>
       </c>
       <c r="G31" t="n" s="0">
-        <v>0.3908</v>
+        <v>0.4523</v>
       </c>
     </row>
     <row r="32">
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="C32" t="n" s="0">
-        <v>30685.0</v>
+        <v>30865.0</v>
       </c>
       <c r="D32" t="n" s="0">
         <v>956.0</v>
@@ -828,10 +828,10 @@
         <v>1478.0</v>
       </c>
       <c r="F32" t="n" s="0">
-        <v>1475.0</v>
+        <v>1478.0</v>
       </c>
       <c r="G32" t="n" s="0">
-        <v>2.5148</v>
+        <v>3.2162</v>
       </c>
     </row>
     <row r="33">
@@ -854,7 +854,7 @@
         <v>2956.0</v>
       </c>
       <c r="G33" t="n" s="0">
-        <v>2.8131</v>
+        <v>3.4605</v>
       </c>
     </row>
     <row r="34">
@@ -877,7 +877,7 @@
         <v>1158.0</v>
       </c>
       <c r="G34" t="n" s="0">
-        <v>1.7032</v>
+        <v>1.9287</v>
       </c>
     </row>
     <row r="35">
@@ -900,7 +900,7 @@
         <v>2316.0</v>
       </c>
       <c r="G35" t="n" s="0">
-        <v>1.9138</v>
+        <v>1.5421</v>
       </c>
     </row>
     <row r="36">
@@ -923,7 +923,7 @@
         <v>850.0</v>
       </c>
       <c r="G36" t="n" s="0">
-        <v>1.6853</v>
+        <v>1.3617</v>
       </c>
     </row>
     <row r="37">
@@ -946,7 +946,7 @@
         <v>1700.0</v>
       </c>
       <c r="G37" t="n" s="0">
-        <v>1.8641</v>
+        <v>0.9535</v>
       </c>
     </row>
     <row r="38">
@@ -957,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="C38" t="n" s="0">
-        <v>23497.0</v>
+        <v>23579.0</v>
       </c>
       <c r="D38" t="n" s="0">
         <v>773.0</v>
@@ -966,10 +966,10 @@
         <v>1386.0</v>
       </c>
       <c r="F38" t="n" s="0">
-        <v>1385.0</v>
+        <v>1386.0</v>
       </c>
       <c r="G38" t="n" s="0">
-        <v>2.1207</v>
+        <v>2.3912</v>
       </c>
     </row>
     <row r="39">
@@ -992,7 +992,7 @@
         <v>2772.0</v>
       </c>
       <c r="G39" t="n" s="0">
-        <v>1.8958</v>
+        <v>1.5447</v>
       </c>
     </row>
     <row r="40">
@@ -1003,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="C40" t="n" s="0">
-        <v>34448.0</v>
+        <v>34782.0</v>
       </c>
       <c r="D40" t="n" s="0">
         <v>996.0</v>
@@ -1012,10 +1012,10 @@
         <v>1498.0</v>
       </c>
       <c r="F40" t="n" s="0">
-        <v>1493.0</v>
+        <v>1498.0</v>
       </c>
       <c r="G40" t="n" s="0">
-        <v>2.2367</v>
+        <v>2.5822</v>
       </c>
     </row>
     <row r="41">
@@ -1038,7 +1038,7 @@
         <v>2996.0</v>
       </c>
       <c r="G41" t="n" s="0">
-        <v>2.0127</v>
+        <v>1.7916</v>
       </c>
     </row>
     <row r="42">
@@ -1061,7 +1061,7 @@
         <v>892.0</v>
       </c>
       <c r="G42" t="n" s="0">
-        <v>1.3953</v>
+        <v>1.6502</v>
       </c>
     </row>
     <row r="43">
@@ -1084,7 +1084,7 @@
         <v>1784.0</v>
       </c>
       <c r="G43" t="n" s="0">
-        <v>1.3285</v>
+        <v>1.0333</v>
       </c>
     </row>
     <row r="44">
@@ -1107,7 +1107,7 @@
         <v>678.0</v>
       </c>
       <c r="G44" t="n" s="0">
-        <v>1.2247</v>
+        <v>1.1184</v>
       </c>
     </row>
     <row r="45">
@@ -1130,7 +1130,7 @@
         <v>1356.0</v>
       </c>
       <c r="G45" t="n" s="0">
-        <v>0.9672</v>
+        <v>0.7144</v>
       </c>
     </row>
     <row r="46">
@@ -1141,7 +1141,7 @@
         <v>7</v>
       </c>
       <c r="C46" t="n" s="0">
-        <v>0.0</v>
+        <v>26292.0</v>
       </c>
       <c r="D46" t="n" s="0">
         <v>865.0</v>
@@ -1150,10 +1150,10 @@
         <v>1432.0</v>
       </c>
       <c r="F46" t="n" s="0">
-        <v>0.0</v>
+        <v>1432.0</v>
       </c>
       <c r="G46" t="n" s="0">
-        <v>0.7628</v>
+        <v>2.753</v>
       </c>
     </row>
     <row r="47">
@@ -1176,7 +1176,7 @@
         <v>2864.0</v>
       </c>
       <c r="G47" t="n" s="0">
-        <v>1.8687</v>
+        <v>1.5457</v>
       </c>
     </row>
     <row r="48">
@@ -1199,7 +1199,7 @@
         <v>1346.0</v>
       </c>
       <c r="G48" t="n" s="0">
-        <v>2.1062</v>
+        <v>2.3949</v>
       </c>
     </row>
     <row r="49">
@@ -1222,7 +1222,7 @@
         <v>2692.0</v>
       </c>
       <c r="G49" t="n" s="0">
-        <v>1.7268</v>
+        <v>1.6001</v>
       </c>
     </row>
     <row r="50">
@@ -1245,7 +1245,7 @@
         <v>698.0</v>
       </c>
       <c r="G50" t="n" s="0">
-        <v>1.3638</v>
+        <v>1.1566</v>
       </c>
     </row>
     <row r="51">
@@ -1268,7 +1268,7 @@
         <v>1396.0</v>
       </c>
       <c r="G51" t="n" s="0">
-        <v>0.9099</v>
+        <v>0.7016</v>
       </c>
     </row>
     <row r="52">
@@ -1279,7 +1279,7 @@
         <v>7</v>
       </c>
       <c r="C52" t="n" s="0">
-        <v>38375.0</v>
+        <v>38856.0</v>
       </c>
       <c r="D52" t="n" s="0">
         <v>1141.0</v>
@@ -1288,10 +1288,10 @@
         <v>1570.0</v>
       </c>
       <c r="F52" t="n" s="0">
-        <v>1562.0</v>
+        <v>1570.0</v>
       </c>
       <c r="G52" t="n" s="0">
-        <v>2.7936</v>
+        <v>2.553</v>
       </c>
     </row>
     <row r="53">
@@ -1314,7 +1314,7 @@
         <v>3140.0</v>
       </c>
       <c r="G53" t="n" s="0">
-        <v>2.3294</v>
+        <v>1.827</v>
       </c>
     </row>
     <row r="54">
@@ -1325,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="C54" t="n" s="0">
-        <v>36839.0</v>
+        <v>37138.0</v>
       </c>
       <c r="D54" t="n" s="0">
         <v>1094.0</v>
@@ -1334,10 +1334,10 @@
         <v>1547.0</v>
       </c>
       <c r="F54" t="n" s="0">
-        <v>1537.0</v>
+        <v>1547.0</v>
       </c>
       <c r="G54" t="n" s="0">
-        <v>2.5585</v>
+        <v>2.2739</v>
       </c>
     </row>
     <row r="55">
@@ -1360,7 +1360,7 @@
         <v>3094.0</v>
       </c>
       <c r="G55" t="n" s="0">
-        <v>1.7152</v>
+        <v>1.8458</v>
       </c>
     </row>
     <row r="56">
@@ -1371,7 +1371,7 @@
         <v>7</v>
       </c>
       <c r="C56" t="n" s="0">
-        <v>0.0</v>
+        <v>34510.0</v>
       </c>
       <c r="D56" t="n" s="0">
         <v>1029.0</v>
@@ -1380,10 +1380,10 @@
         <v>1514.0</v>
       </c>
       <c r="F56" t="n" s="0">
-        <v>0.0</v>
+        <v>1514.0</v>
       </c>
       <c r="G56" t="n" s="0">
-        <v>0.504</v>
+        <v>2.0377</v>
       </c>
     </row>
     <row r="57">
@@ -1406,7 +1406,7 @@
         <v>3028.0</v>
       </c>
       <c r="G57" t="n" s="0">
-        <v>2.5646</v>
+        <v>1.7439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>